<commit_message>
Added OutputVolumeMean(...) function which outputs the total volume density at each step of a specified multifab to a specified file.
</commit_message>
<xml_diff>
--- a/exec/immersedIons/Electrolyte_Data.xlsx
+++ b/exec/immersedIons/Electrolyte_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -775,28 +775,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,6 +842,8 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1007,19 +1022,30 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
       <c r="C9" s="3"/>
+      <c r="D9" s="0"/>
       <c r="E9" s="4"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
+      <c r="J9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B10" s="0"/>
       <c r="C10" s="3"/>
+      <c r="D10" s="0"/>
       <c r="E10" s="4"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
+      <c r="J10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -1111,11 +1137,17 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
       <c r="C14" s="3"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,6 +1171,7 @@
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B16" s="0"/>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,7 +1284,15 @@
         <v>0.0058</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+    </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
       <c r="G22" s="9" t="s">
         <v>50</v>
       </c>
@@ -1265,6 +1306,9 @@
         <v>6.0221409E+023</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+    </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>52</v>
@@ -1288,7 +1332,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1303,26 +1347,26 @@
   </sheetPr>
   <dimension ref="A2:V50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.53"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2204,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>